<commit_message>
Update academic schedule template: Revised formatting and structure for improved clarity and usability.
</commit_message>
<xml_diff>
--- a/public/templates/academic_schedules.xlsx
+++ b/public/templates/academic_schedules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\dev\pontiapp-laravel\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DF435A-F040-44BF-8A83-791BD16B29DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8DA7AE-CCEE-4797-A804-85F6DA3F08E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="865" xr2:uid="{9259999E-EE99-4889-B6AC-1B64A662CC4C}"/>
   </bookViews>
@@ -207,7 +207,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -262,9 +262,6 @@
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1229,8 +1226,8 @@
   <dimension ref="A1:AA802"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A765" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J749" sqref="J749:AA800"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M4" sqref="K3:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -21549,7 +21546,6 @@
       <c r="B750" s="16"/>
       <c r="C750" s="16"/>
       <c r="D750" s="2"/>
-      <c r="G750" s="19"/>
       <c r="P750" s="17"/>
       <c r="Q750" s="17"/>
       <c r="R750" s="17">
@@ -21577,7 +21573,6 @@
       <c r="B751" s="16"/>
       <c r="C751" s="16"/>
       <c r="D751" s="2"/>
-      <c r="G751" s="19"/>
       <c r="P751" s="17"/>
       <c r="Q751" s="17"/>
       <c r="R751" s="17">
@@ -21605,7 +21600,6 @@
       <c r="B752" s="16"/>
       <c r="C752" s="16"/>
       <c r="D752" s="2"/>
-      <c r="G752" s="19"/>
       <c r="P752" s="17"/>
       <c r="Q752" s="17"/>
       <c r="R752" s="17">
@@ -21633,7 +21627,6 @@
       <c r="B753" s="16"/>
       <c r="C753" s="16"/>
       <c r="D753" s="2"/>
-      <c r="G753" s="19"/>
       <c r="P753" s="17"/>
       <c r="Q753" s="17"/>
       <c r="R753" s="17">
@@ -21661,7 +21654,6 @@
       <c r="B754" s="16"/>
       <c r="C754" s="16"/>
       <c r="D754" s="2"/>
-      <c r="G754" s="19"/>
       <c r="P754" s="17"/>
       <c r="Q754" s="17"/>
       <c r="R754" s="17">
@@ -21689,7 +21681,6 @@
       <c r="B755" s="16"/>
       <c r="C755" s="16"/>
       <c r="D755" s="2"/>
-      <c r="G755" s="19"/>
       <c r="P755" s="17"/>
       <c r="Q755" s="17"/>
       <c r="R755" s="17">
@@ -21717,7 +21708,6 @@
       <c r="B756" s="16"/>
       <c r="C756" s="16"/>
       <c r="D756" s="2"/>
-      <c r="G756" s="19"/>
       <c r="P756" s="17"/>
       <c r="Q756" s="17"/>
       <c r="R756" s="17">
@@ -21745,7 +21735,6 @@
       <c r="B757" s="16"/>
       <c r="C757" s="16"/>
       <c r="D757" s="2"/>
-      <c r="G757" s="19"/>
       <c r="P757" s="17"/>
       <c r="Q757" s="17"/>
       <c r="R757" s="17">
@@ -21773,7 +21762,6 @@
       <c r="B758" s="16"/>
       <c r="C758" s="16"/>
       <c r="D758" s="2"/>
-      <c r="G758" s="19"/>
       <c r="P758" s="17"/>
       <c r="Q758" s="17"/>
       <c r="R758" s="17">
@@ -21801,7 +21789,6 @@
       <c r="B759" s="16"/>
       <c r="C759" s="16"/>
       <c r="D759" s="2"/>
-      <c r="G759" s="19"/>
       <c r="P759" s="17"/>
       <c r="Q759" s="17"/>
       <c r="R759" s="17">
@@ -21829,7 +21816,6 @@
       <c r="B760" s="16"/>
       <c r="C760" s="16"/>
       <c r="D760" s="2"/>
-      <c r="G760" s="19"/>
       <c r="P760" s="17"/>
       <c r="Q760" s="17"/>
       <c r="R760" s="17">
@@ -21857,7 +21843,6 @@
       <c r="B761" s="16"/>
       <c r="C761" s="16"/>
       <c r="D761" s="2"/>
-      <c r="G761" s="19"/>
       <c r="P761" s="17"/>
       <c r="Q761" s="17"/>
       <c r="R761" s="17">
@@ -21885,7 +21870,6 @@
       <c r="B762" s="16"/>
       <c r="C762" s="16"/>
       <c r="D762" s="2"/>
-      <c r="G762" s="19"/>
       <c r="P762" s="17"/>
       <c r="Q762" s="17"/>
       <c r="R762" s="17">
@@ -21913,7 +21897,6 @@
       <c r="B763" s="16"/>
       <c r="C763" s="16"/>
       <c r="D763" s="2"/>
-      <c r="G763" s="19"/>
       <c r="P763" s="17"/>
       <c r="Q763" s="17"/>
       <c r="R763" s="17">
@@ -21941,7 +21924,6 @@
       <c r="B764" s="16"/>
       <c r="C764" s="16"/>
       <c r="D764" s="2"/>
-      <c r="G764" s="19"/>
       <c r="P764" s="17"/>
       <c r="Q764" s="17"/>
       <c r="R764" s="17">
@@ -21969,7 +21951,6 @@
       <c r="B765" s="16"/>
       <c r="C765" s="16"/>
       <c r="D765" s="2"/>
-      <c r="G765" s="19"/>
       <c r="P765" s="17"/>
       <c r="Q765" s="17"/>
       <c r="R765" s="17">
@@ -21997,7 +21978,6 @@
       <c r="B766" s="16"/>
       <c r="C766" s="16"/>
       <c r="D766" s="2"/>
-      <c r="G766" s="19"/>
       <c r="P766" s="17"/>
       <c r="Q766" s="17"/>
       <c r="R766" s="17">
@@ -22025,7 +22005,6 @@
       <c r="B767" s="16"/>
       <c r="C767" s="16"/>
       <c r="D767" s="2"/>
-      <c r="G767" s="19"/>
       <c r="P767" s="17"/>
       <c r="Q767" s="17"/>
       <c r="R767" s="17">
@@ -22053,7 +22032,6 @@
       <c r="B768" s="16"/>
       <c r="C768" s="16"/>
       <c r="D768" s="2"/>
-      <c r="G768" s="19"/>
       <c r="P768" s="17"/>
       <c r="Q768" s="17"/>
       <c r="R768" s="17">
@@ -22081,7 +22059,6 @@
       <c r="B769" s="16"/>
       <c r="C769" s="16"/>
       <c r="D769" s="2"/>
-      <c r="G769" s="19"/>
       <c r="P769" s="17"/>
       <c r="Q769" s="17"/>
       <c r="R769" s="17">
@@ -22109,7 +22086,6 @@
       <c r="B770" s="16"/>
       <c r="C770" s="16"/>
       <c r="D770" s="2"/>
-      <c r="G770" s="19"/>
       <c r="P770" s="17"/>
       <c r="Q770" s="17"/>
       <c r="R770" s="17">
@@ -22137,7 +22113,6 @@
       <c r="B771" s="16"/>
       <c r="C771" s="16"/>
       <c r="D771" s="2"/>
-      <c r="G771" s="19"/>
       <c r="P771" s="17"/>
       <c r="Q771" s="17"/>
       <c r="R771" s="17">
@@ -22165,7 +22140,6 @@
       <c r="B772" s="16"/>
       <c r="C772" s="16"/>
       <c r="D772" s="2"/>
-      <c r="G772" s="19"/>
       <c r="P772" s="17"/>
       <c r="Q772" s="17"/>
       <c r="R772" s="17">
@@ -22193,7 +22167,6 @@
       <c r="B773" s="16"/>
       <c r="C773" s="16"/>
       <c r="D773" s="2"/>
-      <c r="G773" s="19"/>
       <c r="P773" s="17"/>
       <c r="Q773" s="17"/>
       <c r="R773" s="17">
@@ -22221,7 +22194,6 @@
       <c r="B774" s="16"/>
       <c r="C774" s="16"/>
       <c r="D774" s="2"/>
-      <c r="G774" s="19"/>
       <c r="P774" s="17"/>
       <c r="Q774" s="17"/>
       <c r="R774" s="17">
@@ -22249,7 +22221,6 @@
       <c r="B775" s="16"/>
       <c r="C775" s="16"/>
       <c r="D775" s="2"/>
-      <c r="G775" s="19"/>
       <c r="P775" s="17"/>
       <c r="Q775" s="17"/>
       <c r="R775" s="17">
@@ -22277,7 +22248,6 @@
       <c r="B776" s="16"/>
       <c r="C776" s="16"/>
       <c r="D776" s="2"/>
-      <c r="G776" s="19"/>
       <c r="P776" s="17"/>
       <c r="Q776" s="17"/>
       <c r="R776" s="17">
@@ -22305,7 +22275,6 @@
       <c r="B777" s="16"/>
       <c r="C777" s="16"/>
       <c r="D777" s="2"/>
-      <c r="G777" s="19"/>
       <c r="P777" s="17"/>
       <c r="Q777" s="17"/>
       <c r="R777" s="17">
@@ -22333,7 +22302,6 @@
       <c r="B778" s="16"/>
       <c r="C778" s="16"/>
       <c r="D778" s="2"/>
-      <c r="G778" s="19"/>
       <c r="P778" s="17"/>
       <c r="Q778" s="17"/>
       <c r="R778" s="17">
@@ -22361,7 +22329,6 @@
       <c r="B779" s="16"/>
       <c r="C779" s="16"/>
       <c r="D779" s="2"/>
-      <c r="G779" s="19"/>
       <c r="P779" s="17"/>
       <c r="Q779" s="17"/>
       <c r="R779" s="17">
@@ -22389,7 +22356,6 @@
       <c r="B780" s="16"/>
       <c r="C780" s="16"/>
       <c r="D780" s="2"/>
-      <c r="G780" s="19"/>
       <c r="P780" s="17"/>
       <c r="Q780" s="17"/>
       <c r="R780" s="17">
@@ -22417,7 +22383,6 @@
       <c r="B781" s="16"/>
       <c r="C781" s="16"/>
       <c r="D781" s="2"/>
-      <c r="G781" s="19"/>
       <c r="P781" s="17"/>
       <c r="Q781" s="17"/>
       <c r="R781" s="17">
@@ -22445,7 +22410,6 @@
       <c r="B782" s="16"/>
       <c r="C782" s="16"/>
       <c r="D782" s="2"/>
-      <c r="G782" s="19"/>
       <c r="P782" s="17"/>
       <c r="Q782" s="17"/>
       <c r="R782" s="17">
@@ -22473,7 +22437,6 @@
       <c r="B783" s="16"/>
       <c r="C783" s="16"/>
       <c r="D783" s="2"/>
-      <c r="G783" s="19"/>
       <c r="P783" s="17"/>
       <c r="Q783" s="17"/>
       <c r="R783" s="17">
@@ -22501,7 +22464,6 @@
       <c r="B784" s="16"/>
       <c r="C784" s="16"/>
       <c r="D784" s="2"/>
-      <c r="G784" s="19"/>
       <c r="P784" s="17"/>
       <c r="Q784" s="17"/>
       <c r="R784" s="17">
@@ -22529,7 +22491,6 @@
       <c r="B785" s="16"/>
       <c r="C785" s="16"/>
       <c r="D785" s="2"/>
-      <c r="G785" s="19"/>
       <c r="P785" s="17"/>
       <c r="Q785" s="17"/>
       <c r="R785" s="17">
@@ -22557,7 +22518,6 @@
       <c r="B786" s="16"/>
       <c r="C786" s="16"/>
       <c r="D786" s="2"/>
-      <c r="G786" s="19"/>
       <c r="P786" s="17"/>
       <c r="Q786" s="17"/>
       <c r="R786" s="17">
@@ -22585,7 +22545,6 @@
       <c r="B787" s="16"/>
       <c r="C787" s="16"/>
       <c r="D787" s="2"/>
-      <c r="G787" s="19"/>
       <c r="P787" s="17"/>
       <c r="Q787" s="17"/>
       <c r="R787" s="17">
@@ -22613,7 +22572,6 @@
       <c r="B788" s="16"/>
       <c r="C788" s="16"/>
       <c r="D788" s="2"/>
-      <c r="G788" s="19"/>
       <c r="P788" s="17"/>
       <c r="Q788" s="17"/>
       <c r="R788" s="17">
@@ -22641,7 +22599,6 @@
       <c r="B789" s="16"/>
       <c r="C789" s="16"/>
       <c r="D789" s="2"/>
-      <c r="G789" s="19"/>
       <c r="P789" s="17"/>
       <c r="Q789" s="17"/>
       <c r="R789" s="17">
@@ -22669,7 +22626,6 @@
       <c r="B790" s="16"/>
       <c r="C790" s="16"/>
       <c r="D790" s="2"/>
-      <c r="G790" s="19"/>
       <c r="P790" s="17"/>
       <c r="Q790" s="17"/>
       <c r="R790" s="17">
@@ -22697,7 +22653,6 @@
       <c r="B791" s="16"/>
       <c r="C791" s="16"/>
       <c r="D791" s="2"/>
-      <c r="G791" s="19"/>
       <c r="P791" s="17"/>
       <c r="Q791" s="17"/>
       <c r="R791" s="17">
@@ -22725,7 +22680,6 @@
       <c r="B792" s="16"/>
       <c r="C792" s="16"/>
       <c r="D792" s="2"/>
-      <c r="G792" s="19"/>
       <c r="P792" s="17"/>
       <c r="Q792" s="17"/>
       <c r="R792" s="17">
@@ -22753,7 +22707,6 @@
       <c r="B793" s="16"/>
       <c r="C793" s="16"/>
       <c r="D793" s="2"/>
-      <c r="G793" s="19"/>
       <c r="P793" s="17"/>
       <c r="Q793" s="17"/>
       <c r="R793" s="17">
@@ -22781,7 +22734,6 @@
       <c r="B794" s="16"/>
       <c r="C794" s="16"/>
       <c r="D794" s="2"/>
-      <c r="G794" s="19"/>
       <c r="P794" s="17"/>
       <c r="Q794" s="17"/>
       <c r="R794" s="17">
@@ -22809,7 +22761,6 @@
       <c r="B795" s="16"/>
       <c r="C795" s="16"/>
       <c r="D795" s="2"/>
-      <c r="G795" s="19"/>
       <c r="P795" s="17"/>
       <c r="Q795" s="17"/>
       <c r="R795" s="17">
@@ -22837,7 +22788,6 @@
       <c r="B796" s="16"/>
       <c r="C796" s="16"/>
       <c r="D796" s="2"/>
-      <c r="G796" s="19"/>
       <c r="P796" s="17"/>
       <c r="Q796" s="17"/>
       <c r="R796" s="17">
@@ -22865,7 +22815,6 @@
       <c r="B797" s="16"/>
       <c r="C797" s="16"/>
       <c r="D797" s="2"/>
-      <c r="G797" s="19"/>
       <c r="P797" s="17"/>
       <c r="Q797" s="17"/>
       <c r="R797" s="17">
@@ -22893,7 +22842,6 @@
       <c r="B798" s="16"/>
       <c r="C798" s="16"/>
       <c r="D798" s="2"/>
-      <c r="G798" s="19"/>
       <c r="P798" s="17"/>
       <c r="Q798" s="17"/>
       <c r="R798" s="17">
@@ -22921,7 +22869,6 @@
       <c r="B799" s="16"/>
       <c r="C799" s="16"/>
       <c r="D799" s="2"/>
-      <c r="G799" s="19"/>
       <c r="P799" s="17"/>
       <c r="Q799" s="17"/>
       <c r="R799" s="17">
@@ -22949,7 +22896,6 @@
       <c r="B800" s="16"/>
       <c r="C800" s="16"/>
       <c r="D800" s="2"/>
-      <c r="G800" s="19"/>
       <c r="P800" s="17"/>
       <c r="Q800" s="17"/>
       <c r="R800" s="17">
@@ -23012,26 +22958,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="37ecd0a5-71f9-4c5b-b3cf-7cf352144f46" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5f24e66c-f230-426f-9d92-48a8e3615176">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101003028B5769EBDAB49A096EDFC08236B01" ma:contentTypeVersion="13" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="6fbdc2ccc97b359d0bb416e33fed9603">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5f24e66c-f230-426f-9d92-48a8e3615176" xmlns:ns3="37ecd0a5-71f9-4c5b-b3cf-7cf352144f46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b4de5ee9f4be5784968e1025018b835a" ns2:_="" ns3:_="">
     <xsd:import namespace="5f24e66c-f230-426f-9d92-48a8e3615176"/>
@@ -23238,26 +23164,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F00E7468-70B4-4491-9935-CDDA442F9D0A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="37ecd0a5-71f9-4c5b-b3cf-7cf352144f46"/>
-    <ds:schemaRef ds:uri="5f24e66c-f230-426f-9d92-48a8e3615176"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4E038F5-418A-45E5-8538-C7BCB9CD7E3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="37ecd0a5-71f9-4c5b-b3cf-7cf352144f46" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5f24e66c-f230-426f-9d92-48a8e3615176">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8592BED-EFEC-482B-BD9C-97A2EE183974}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23274,4 +23201,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4E038F5-418A-45E5-8538-C7BCB9CD7E3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F00E7468-70B4-4491-9935-CDDA442F9D0A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="37ecd0a5-71f9-4c5b-b3cf-7cf352144f46"/>
+    <ds:schemaRef ds:uri="5f24e66c-f230-426f-9d92-48a8e3615176"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>